<commit_message>
Add fields to blank row
</commit_message>
<xml_diff>
--- a/test_transformed.xlsx
+++ b/test_transformed.xlsx
@@ -397,399 +397,360 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>incidentId</v>
+      </c>
+      <c r="B1" t="str">
+        <v>type</v>
+      </c>
+      <c r="C1" t="str">
+        <v>location.type</v>
+      </c>
+      <c r="D1" t="str">
+        <v>advisories.type</v>
+      </c>
+      <c r="E1" t="str">
+        <v>responders.agency.personnel.name</v>
+      </c>
+      <c r="F1" t="str">
         <v>employeeId</v>
       </c>
-      <c r="B1" t="str">
+      <c r="G1" t="str">
         <v>firstName</v>
       </c>
-      <c r="C1" t="str">
+      <c r="H1" t="str">
         <v>personalInfo.dateOfBirth</v>
       </c>
-      <c r="D1" t="str">
+      <c r="I1" t="str">
         <v>personalInfo.phoneNumber</v>
       </c>
-      <c r="E1" t="str">
+      <c r="J1" t="str">
         <v>personalInfo.emergencyContact</v>
       </c>
-      <c r="F1" t="str">
+      <c r="K1" t="str">
         <v>lastName</v>
       </c>
-      <c r="G1" t="str">
+      <c r="L1" t="str">
         <v>email</v>
       </c>
-      <c r="H1" t="str">
+      <c r="M1" t="str">
         <v>employments.performanceReviews.reviewId</v>
       </c>
-      <c r="I1" t="str">
+      <c r="N1" t="str">
         <v>employments.performanceReviews.metrics.metricName</v>
       </c>
-      <c r="J1" t="str">
+      <c r="O1" t="str">
         <v>employments.performanceReviews.metrics.score</v>
       </c>
-      <c r="K1" t="str">
+      <c r="P1" t="str">
         <v>employments.performanceReviews.reviewDate</v>
       </c>
-      <c r="L1" t="str">
+      <c r="Q1" t="str">
         <v>employments.yearsOfService</v>
       </c>
-      <c r="M1" t="str">
+      <c r="R1" t="str">
         <v>employments.department</v>
       </c>
-      <c r="N1" t="str">
+      <c r="S1" t="str">
         <v>skills.skillName</v>
       </c>
-      <c r="O1" t="str">
+      <c r="T1" t="str">
         <v>skills.proficiencyLevel</v>
       </c>
-      <c r="P1" t="str">
+      <c r="U1" t="str">
         <v>trainingHistory.courseName</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="V1" t="str">
         <v>trainingHistory.completionDate</v>
       </c>
-      <c r="R1" t="str">
+      <c r="W1" t="str">
         <v>trainingHistory.certifications.certificationName</v>
       </c>
-      <c r="S1" t="str">
+      <c r="X1" t="str">
         <v>trainingHistory.certifications.issueDate</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>EMP-2024-001</v>
+        <v/>
       </c>
       <c r="B2" t="str">
-        <v>Sarah</v>
+        <v/>
       </c>
       <c r="C2" t="str">
-        <v>1990-03-15</v>
+        <v/>
       </c>
       <c r="D2" t="str">
-        <v>+1-555-0123</v>
+        <v/>
       </c>
       <c r="E2" t="str">
-        <v>John Mitchell (Spouse)</v>
-      </c>
-      <c r="F2" t="str">
-        <v>Johnson</v>
-      </c>
-      <c r="G2" t="str">
-        <v>sarah.johnson@company.com</v>
-      </c>
-      <c r="H2" t="str">
-        <v>REV-2024-Q1</v>
-      </c>
-      <c r="I2" t="str">
-        <v>Technical Skills</v>
-      </c>
-      <c r="J2" t="str">
-        <v>4.5</v>
-      </c>
-      <c r="K2" t="str">
-        <v>2024-03-15</v>
-      </c>
-      <c r="L2">
-        <v>3</v>
-      </c>
-      <c r="M2" t="str">
-        <v>Software Engineering</v>
-      </c>
-      <c r="N2" t="str">
-        <v>JavaScript</v>
-      </c>
-      <c r="O2" t="str">
-        <v>Expert</v>
-      </c>
-      <c r="P2" t="str">
-        <v>Advanced Leadership Development</v>
-      </c>
-      <c r="Q2" t="str">
-        <v>2024-02-28</v>
-      </c>
-      <c r="R2" t="str">
-        <v>Certified Scrum Master</v>
-      </c>
-      <c r="S2" t="str">
-        <v>2024-01-15</v>
+        <v/>
       </c>
     </row>
     <row r="3">
-      <c r="I3" t="str">
-        <v>Communication</v>
-      </c>
-      <c r="J3" t="str">
-        <v>4.0</v>
-      </c>
-      <c r="N3" t="str">
-        <v>Project Management</v>
-      </c>
-      <c r="O3" t="str">
-        <v>Intermediate</v>
-      </c>
-      <c r="R3" t="str">
-        <v>AWS Solutions Architect</v>
-      </c>
-      <c r="S3" t="str">
-        <v>2023-11-20</v>
+      <c r="A3" t="str">
+        <v/>
+      </c>
+      <c r="B3" t="str">
+        <v/>
+      </c>
+      <c r="C3" t="str">
+        <v/>
+      </c>
+      <c r="D3" t="str">
+        <v/>
+      </c>
+      <c r="E3" t="str">
+        <v/>
       </c>
     </row>
     <row r="4">
-      <c r="H4" t="str">
-        <v>REV-2024-Q2</v>
-      </c>
-      <c r="I4" t="str">
-        <v>Technical Skills</v>
-      </c>
-      <c r="J4" t="str">
-        <v>4.5</v>
-      </c>
-      <c r="K4" t="str">
-        <v>2024-03-15</v>
-      </c>
-      <c r="P4" t="str">
-        <v>Advanced Leadership Development 2</v>
-      </c>
-      <c r="Q4" t="str">
-        <v>2024-02-28</v>
-      </c>
-      <c r="R4" t="str">
-        <v>Certified Scrum Master</v>
-      </c>
-      <c r="S4" t="str">
-        <v>2024-01-15</v>
+      <c r="A4" t="str">
+        <v/>
+      </c>
+      <c r="B4" t="str">
+        <v/>
+      </c>
+      <c r="C4" t="str">
+        <v/>
+      </c>
+      <c r="D4" t="str">
+        <v/>
+      </c>
+      <c r="E4" t="str">
+        <v/>
       </c>
     </row>
     <row r="5">
-      <c r="I5" t="str">
-        <v>Communication</v>
-      </c>
-      <c r="J5" t="str">
-        <v>4.0</v>
-      </c>
-      <c r="R5" t="str">
-        <v>AWS Solutions Architect</v>
-      </c>
-      <c r="S5" t="str">
-        <v>2023-11-20</v>
+      <c r="A5" t="str">
+        <v/>
+      </c>
+      <c r="B5" t="str">
+        <v/>
+      </c>
+      <c r="C5" t="str">
+        <v/>
+      </c>
+      <c r="D5" t="str">
+        <v/>
+      </c>
+      <c r="E5" t="str">
+        <v/>
       </c>
     </row>
     <row r="6">
-      <c r="H6" t="str">
-        <v>REV-2024-Q1</v>
-      </c>
-      <c r="I6" t="str">
-        <v>Technical Skills</v>
-      </c>
-      <c r="J6" t="str">
-        <v>4.5</v>
-      </c>
-      <c r="K6" t="str">
-        <v>2024-03-15</v>
-      </c>
-      <c r="L6">
-        <v>3</v>
-      </c>
-      <c r="M6" t="str">
-        <v>Prompt Engineering</v>
+      <c r="A6" t="str">
+        <v/>
+      </c>
+      <c r="B6" t="str">
+        <v/>
+      </c>
+      <c r="C6" t="str">
+        <v/>
+      </c>
+      <c r="D6" t="str">
+        <v/>
+      </c>
+      <c r="E6" t="str">
+        <v/>
       </c>
     </row>
     <row r="7">
-      <c r="I7" t="str">
-        <v>Communication</v>
-      </c>
-      <c r="J7" t="str">
-        <v>4.0</v>
+      <c r="A7" t="str">
+        <v/>
+      </c>
+      <c r="B7" t="str">
+        <v/>
+      </c>
+      <c r="C7" t="str">
+        <v/>
+      </c>
+      <c r="D7" t="str">
+        <v/>
+      </c>
+      <c r="E7" t="str">
+        <v/>
       </c>
     </row>
     <row r="8">
-      <c r="H8" t="str">
-        <v>REV-2024-Q2</v>
-      </c>
-      <c r="I8" t="str">
-        <v>Technical Skills</v>
-      </c>
-      <c r="J8" t="str">
-        <v>4.5</v>
-      </c>
-      <c r="K8" t="str">
-        <v>2024-03-15</v>
+      <c r="A8" t="str">
+        <v/>
+      </c>
+      <c r="B8" t="str">
+        <v/>
+      </c>
+      <c r="C8" t="str">
+        <v/>
+      </c>
+      <c r="D8" t="str">
+        <v/>
+      </c>
+      <c r="E8" t="str">
+        <v/>
       </c>
     </row>
     <row r="9">
-      <c r="I9" t="str">
-        <v>Communication</v>
-      </c>
-      <c r="J9" t="str">
-        <v>4.0</v>
+      <c r="A9" t="str">
+        <v/>
+      </c>
+      <c r="B9" t="str">
+        <v/>
+      </c>
+      <c r="C9" t="str">
+        <v/>
+      </c>
+      <c r="D9" t="str">
+        <v/>
+      </c>
+      <c r="E9" t="str">
+        <v/>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>EMP-2024-002</v>
+        <v/>
       </c>
       <c r="B10" t="str">
-        <v>Michael</v>
+        <v/>
       </c>
       <c r="C10" t="str">
-        <v>1985-07-22</v>
+        <v/>
       </c>
       <c r="D10" t="str">
-        <v>+1-555-0456</v>
+        <v/>
       </c>
       <c r="E10" t="str">
-        <v>Lisa Chen (Sister)</v>
-      </c>
-      <c r="F10" t="str">
-        <v>Rodriguez</v>
-      </c>
-      <c r="G10" t="str">
-        <v>michael.rodriguez@company.com</v>
-      </c>
-      <c r="H10" t="str">
-        <v>REV-2024-Q1</v>
-      </c>
-      <c r="I10" t="str">
-        <v>Technical Skills</v>
-      </c>
-      <c r="J10" t="str">
-        <v>4.5</v>
-      </c>
-      <c r="K10" t="str">
-        <v>2024-03-15</v>
-      </c>
-      <c r="L10">
-        <v>3</v>
-      </c>
-      <c r="M10" t="str">
-        <v>Software Engineering</v>
-      </c>
-      <c r="N10" t="str">
-        <v>Employee Relations</v>
-      </c>
-      <c r="O10" t="str">
-        <v>Expert</v>
-      </c>
-      <c r="P10" t="str">
-        <v>Diversity and Inclusion Workshop</v>
-      </c>
-      <c r="Q10" t="str">
-        <v>2024-01-10</v>
-      </c>
-      <c r="R10" t="str">
-        <v>PHR Certification</v>
-      </c>
-      <c r="S10" t="str">
-        <v>2023-08-15</v>
+        <v/>
       </c>
     </row>
     <row r="11">
-      <c r="I11" t="str">
-        <v>Communication</v>
-      </c>
-      <c r="J11" t="str">
-        <v>4.0</v>
-      </c>
-      <c r="N11" t="str">
-        <v>Data Analysis</v>
-      </c>
-      <c r="O11" t="str">
-        <v>Intermediate</v>
-      </c>
-      <c r="P11" t="str">
-        <v>Diversity and Inclusion Workshop 2</v>
-      </c>
-      <c r="Q11" t="str">
-        <v>2024-01-10</v>
-      </c>
-      <c r="R11" t="str">
-        <v>PHR Certification</v>
-      </c>
-      <c r="S11" t="str">
-        <v>2023-08-15</v>
+      <c r="A11" t="str">
+        <v/>
+      </c>
+      <c r="B11" t="str">
+        <v/>
+      </c>
+      <c r="C11" t="str">
+        <v/>
+      </c>
+      <c r="D11" t="str">
+        <v/>
+      </c>
+      <c r="E11" t="str">
+        <v/>
       </c>
     </row>
     <row r="12">
-      <c r="H12" t="str">
-        <v>REV-2024-Q2</v>
-      </c>
-      <c r="I12" t="str">
-        <v>Technical Skills</v>
-      </c>
-      <c r="J12" t="str">
-        <v>4.5</v>
-      </c>
-      <c r="K12" t="str">
-        <v>2024-03-15</v>
+      <c r="A12" t="str">
+        <v/>
+      </c>
+      <c r="B12" t="str">
+        <v/>
+      </c>
+      <c r="C12" t="str">
+        <v/>
+      </c>
+      <c r="D12" t="str">
+        <v/>
+      </c>
+      <c r="E12" t="str">
+        <v/>
       </c>
     </row>
     <row r="13">
-      <c r="I13" t="str">
-        <v>Communication</v>
-      </c>
-      <c r="J13" t="str">
-        <v>4.0</v>
+      <c r="A13" t="str">
+        <v/>
+      </c>
+      <c r="B13" t="str">
+        <v/>
+      </c>
+      <c r="C13" t="str">
+        <v/>
+      </c>
+      <c r="D13" t="str">
+        <v/>
+      </c>
+      <c r="E13" t="str">
+        <v/>
       </c>
     </row>
     <row r="14">
-      <c r="H14" t="str">
-        <v>REV-2024-Q1</v>
-      </c>
-      <c r="I14" t="str">
-        <v>Technical Skills</v>
-      </c>
-      <c r="J14" t="str">
-        <v>4.5</v>
-      </c>
-      <c r="K14" t="str">
-        <v>2024-03-15</v>
-      </c>
-      <c r="L14">
-        <v>3</v>
-      </c>
-      <c r="M14" t="str">
-        <v>Prompt Engineering</v>
+      <c r="A14" t="str">
+        <v/>
+      </c>
+      <c r="B14" t="str">
+        <v/>
+      </c>
+      <c r="C14" t="str">
+        <v/>
+      </c>
+      <c r="D14" t="str">
+        <v/>
+      </c>
+      <c r="E14" t="str">
+        <v/>
       </c>
     </row>
     <row r="15">
-      <c r="I15" t="str">
-        <v>Communication</v>
-      </c>
-      <c r="J15" t="str">
-        <v>4.0</v>
+      <c r="A15" t="str">
+        <v/>
+      </c>
+      <c r="B15" t="str">
+        <v/>
+      </c>
+      <c r="C15" t="str">
+        <v/>
+      </c>
+      <c r="D15" t="str">
+        <v/>
+      </c>
+      <c r="E15" t="str">
+        <v/>
       </c>
     </row>
     <row r="16">
-      <c r="H16" t="str">
-        <v>REV-2024-Q2</v>
-      </c>
-      <c r="I16" t="str">
-        <v>Technical Skills</v>
-      </c>
-      <c r="J16" t="str">
-        <v>4.5</v>
-      </c>
-      <c r="K16" t="str">
-        <v>2024-03-15</v>
+      <c r="A16" t="str">
+        <v/>
+      </c>
+      <c r="B16" t="str">
+        <v/>
+      </c>
+      <c r="C16" t="str">
+        <v/>
+      </c>
+      <c r="D16" t="str">
+        <v/>
+      </c>
+      <c r="E16" t="str">
+        <v/>
       </c>
     </row>
     <row r="17">
-      <c r="I17" t="str">
-        <v>Communication</v>
-      </c>
-      <c r="J17" t="str">
-        <v>4.0</v>
+      <c r="A17" t="str">
+        <v/>
+      </c>
+      <c r="B17" t="str">
+        <v/>
+      </c>
+      <c r="C17" t="str">
+        <v/>
+      </c>
+      <c r="D17" t="str">
+        <v/>
+      </c>
+      <c r="E17" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:S17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:X17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>